<commit_message>
Excel unittest ajout classe planning et user
</commit_message>
<xml_diff>
--- a/projet/unittest/Unittet-KOT-test.xlsx
+++ b/projet/unittest/Unittet-KOT-test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t xml:space="preserve">Test </t>
   </si>
@@ -214,18 +214,42 @@
   <si>
     <t>Error</t>
   </si>
+  <si>
+    <t>DDay (planning)</t>
+  </si>
+  <si>
+    <t>result = planning.DDay()</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> datetime.strftime(today, "%d-%m-%Y")</t>
+  </si>
+  <si>
+    <t>newDDay</t>
+  </si>
+  <si>
+    <t>planning.newDDay()</t>
+  </si>
+  <si>
+    <t>expected Output</t>
+  </si>
+  <si>
+    <t>expected output</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="d\.m"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="d\ m"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="d\ m"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="d\,m"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -284,9 +308,40 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -299,22 +354,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -322,22 +362,22 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -352,15 +392,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -368,30 +400,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -413,17 +445,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -442,13 +466,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,37 +550,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,67 +562,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,37 +574,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -623,6 +587,66 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,6 +675,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -662,6 +719,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -683,24 +749,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -709,175 +757,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -904,10 +928,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
@@ -1177,7 +1201,7 @@
   <dimension ref="A1:Z1083"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6272727272727" defaultRowHeight="15.75" customHeight="1"/>
@@ -2977,10 +3001,18 @@
       <c r="Z56" s="5"/>
     </row>
     <row r="57" customHeight="1" spans="1:26">
-      <c r="A57" s="3"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
+      <c r="A57" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
@@ -3007,8 +3039,12 @@
     <row r="58" customHeight="1" spans="1:26">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
+      <c r="C58" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
@@ -3033,7 +3069,7 @@
       <c r="Z58" s="5"/>
     </row>
     <row r="59" customHeight="1" spans="1:26">
-      <c r="A59" s="3"/>
+      <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -3061,10 +3097,18 @@
       <c r="Z59" s="5"/>
     </row>
     <row r="60" customHeight="1" spans="1:26">
-      <c r="A60" s="3"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
+      <c r="A60" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>

</xml_diff>